<commit_message>
Made Changes to the following VI's: eventMode.vi: Changed the UI and added a pixel map, threshold slider, and user name & description control csvNameGenerate.vi: Changed the output file name to include User name, desc, threshold & time format
Added the following new files:
chkEvntSet.vi: Checks if all the data input by the user is proper or not in eventMode.vi
pixelArray.ctl: Added the pixel array as a control file
allSettings.vi: Added a new UI file for reg map type interface
</commit_message>
<xml_diff>
--- a/Database/Dictionary Commands.xlsx
+++ b/Database/Dictionary Commands.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20354"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FE4673-C55F-4BFE-ABA2-26AB9819F5F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC425A9-6B22-4A0B-898B-3FE6BA32B961}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -159,12 +159,141 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +577,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,738 +1225,738 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="7">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="7">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="7">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="4">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="4">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="4">
         <v>44</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="7">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0</v>
+      </c>
+      <c r="H23" s="8">
+        <v>0</v>
+      </c>
+      <c r="I23" s="8">
+        <v>1</v>
+      </c>
+      <c r="J23" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>